<commit_message>
Second Commit...change in validInvalidLoginTest()....
</commit_message>
<xml_diff>
--- a/src/test/resources/DemoExeData01.xlsx
+++ b/src/test/resources/DemoExeData01.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31909512-FB1F-4500-A45D-72BC7E8C52B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC35E05-C733-4945-ACED-3B9867680FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4872" yWindow="2244" windowWidth="16344" windowHeight="9996" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4872" yWindow="2244" windowWidth="16344" windowHeight="9996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -562,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
com.tutorialninja.pagefactory package rename to com.tutorialninja.pageobjects
</commit_message>
<xml_diff>
--- a/src/test/resources/DemoExeData01.xlsx
+++ b/src/test/resources/DemoExeData01.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543F09A7-4738-4F9F-9185-0172648B6E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DE0264-9448-4755-95F4-FF36163B7CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4872" yWindow="2244" windowWidth="16344" windowHeight="9996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4872" yWindow="2244" windowWidth="16344" windowHeight="9996" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
@@ -198,12 +198,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -511,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,37 +601,37 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -790,8 +790,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{6B163034-FF13-4803-ABC8-B8157652651C}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{EC9BBC80-5442-447F-8938-ECAA6EE533AD}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{EC9BBC80-5442-447F-8938-ECAA6EE533AD}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{C9D6B45F-6FA3-47AC-8790-FFC49969EA43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>